<commit_message>
Changing conversion to class-based converter
</commit_message>
<xml_diff>
--- a/py_convert/ONE_DATA/Oneida_spreadsheet_unicode.xlsx
+++ b/py_convert/ONE_DATA/Oneida_spreadsheet_unicode.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="500" visibility="visible" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1" iterate="0" iterateCount="100" iterateDelta="0.001" refMode="A1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -84,7 +84,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt formatCode="General" numFmtId="164"/>
+  </numFmts>
   <fonts count="8">
     <font>
       <name val="Arial"/>
@@ -126,7 +128,7 @@
       <u val="single"/>
     </font>
     <font>
-      <name val="NotoSans-Regular"/>
+      <name val="Times New Roman"/>
       <charset val="1"/>
       <family val="0"/>
       <sz val="20"/>
@@ -150,36 +152,25 @@
     </border>
   </borders>
   <cellStyleXfs count="6">
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="5">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="7" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -491,176 +482,176 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="24.45" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="3" width="11.52"/>
-    <col customWidth="1" max="2" min="2" style="4" width="82.81"/>
-    <col customWidth="1" max="1025" min="3" style="5" width="11.52"/>
+    <col customWidth="1" max="1" min="1" style="1" width="11.52"/>
+    <col customWidth="1" max="2" min="2" style="2" width="82.81"/>
+    <col customWidth="1" max="1025" min="3" width="11.52"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="24.45" r="1" s="6" spans="1:2">
-      <c r="A1" s="3" t="n">
+    <row customHeight="1" ht="24.45" r="1" s="3" spans="1:2">
+      <c r="A1" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row customHeight="1" ht="24.45" r="2" s="6" spans="1:2">
-      <c r="A2" s="3" t="n">
+    <row customHeight="1" ht="24.45" r="2" s="3" spans="1:2">
+      <c r="A2" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row customHeight="1" ht="24.45" r="3" s="6" spans="1:2">
-      <c r="A3" s="3" t="n">
+    <row customHeight="1" ht="24.45" r="3" s="3" spans="1:2">
+      <c r="A3" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row customHeight="1" ht="24.45" r="4" s="6" spans="1:2">
-      <c r="A4" s="3" t="n">
+    <row customHeight="1" ht="24.45" r="4" s="3" spans="1:2">
+      <c r="A4" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row customHeight="1" ht="24.45" r="5" s="6" spans="1:2">
-      <c r="A5" s="3" t="n">
+    <row customHeight="1" ht="24.45" r="5" s="3" spans="1:2">
+      <c r="A5" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row customHeight="1" ht="24.45" r="6" s="6" spans="1:2">
-      <c r="A6" s="3" t="n">
+    <row customHeight="1" ht="24.45" r="6" s="3" spans="1:2">
+      <c r="A6" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row customHeight="1" ht="24.45" r="7" s="6" spans="1:2">
-      <c r="A7" s="3" t="n">
+    <row customHeight="1" ht="24.45" r="7" s="3" spans="1:2">
+      <c r="A7" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row customHeight="1" ht="24.45" r="8" s="6" spans="1:2">
-      <c r="A8" s="3" t="n">
+    <row customHeight="1" ht="24.45" r="8" s="3" spans="1:2">
+      <c r="A8" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row customHeight="1" ht="24.45" r="9" s="6" spans="1:2">
-      <c r="A9" s="3" t="n">
+    <row customHeight="1" ht="24.45" r="9" s="3" spans="1:2">
+      <c r="A9" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row customHeight="1" ht="24.45" r="10" s="6" spans="1:2">
-      <c r="A10" s="3" t="n">
+    <row customHeight="1" ht="24.45" r="10" s="3" spans="1:2">
+      <c r="A10" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row customHeight="1" ht="24.45" r="11" s="6" spans="1:2">
-      <c r="A11" s="3" t="n">
+    <row customHeight="1" ht="24.45" r="11" s="3" spans="1:2">
+      <c r="A11" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row customHeight="1" ht="24.45" r="12" s="6" spans="1:2">
-      <c r="A12" s="3" t="n">
+    <row customHeight="1" ht="24.45" r="12" s="3" spans="1:2">
+      <c r="A12" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row customHeight="1" ht="24.45" r="13" s="6" spans="1:2">
-      <c r="A13" s="3" t="n">
+    <row customHeight="1" ht="24.45" r="13" s="3" spans="1:2">
+      <c r="A13" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row customHeight="1" ht="24.45" r="14" s="6" spans="1:2">
-      <c r="A14" s="3" t="n">
+    <row customHeight="1" ht="24.45" r="14" s="3" spans="1:2">
+      <c r="A14" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row customHeight="1" ht="24.45" r="15" s="6" spans="1:2">
-      <c r="A15" s="3" t="n">
+    <row customHeight="1" ht="24.45" r="15" s="3" spans="1:2">
+      <c r="A15" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row customHeight="1" ht="24.45" r="16" s="6" spans="1:2">
-      <c r="A16" s="3" t="n">
+    <row customHeight="1" ht="24.45" r="16" s="3" spans="1:2">
+      <c r="A16" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row customHeight="1" ht="24.45" r="17" s="6" spans="1:2">
-      <c r="A17" s="3" t="n">
+    <row customHeight="1" ht="24.45" r="17" s="3" spans="1:2">
+      <c r="A17" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row customHeight="1" ht="24.45" r="18" s="6" spans="1:2">
-      <c r="A18" s="3" t="n">
+    <row customHeight="1" ht="24.45" r="18" s="3" spans="1:2">
+      <c r="A18" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row customHeight="1" ht="45" r="19" s="6" spans="1:2">
-      <c r="A19" s="3" t="n">
+    <row customHeight="1" ht="45" r="19" s="3" spans="1:2">
+      <c r="A19" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row customHeight="1" ht="45" r="20" s="6" spans="1:2">
-      <c r="A20" s="3" t="n">
+    <row customHeight="1" ht="45" r="20" s="3" spans="1:2">
+      <c r="A20" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row customHeight="1" ht="24.45" r="21" s="6" spans="1:2">
-      <c r="A21" s="3" t="n">
+    <row customHeight="1" ht="24.45" r="21" s="3" spans="1:2">
+      <c r="A21" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="4" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>